<commit_message>
changed the test Rail Approach
</commit_message>
<xml_diff>
--- a/resources/excelFiles/Data.xlsx
+++ b/resources/excelFiles/Data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>TC_ID</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>USERNAME</t>
+  </si>
+  <si>
+    <t>loginWithValidCredentialsViral</t>
   </si>
 </sst>
 </file>
@@ -125,10 +128,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,12 +487,20 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -505,6 +519,9 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>